<commit_message>
Designs finalizados e HTML/CSS iniciado.
</commit_message>
<xml_diff>
--- a/Documentação/Fibonacci e Burndown.xlsx
+++ b/Documentação/Fibonacci e Burndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheus\OneDrive\Área de Trabalho\Sempiternal\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B82A1C-5C2F-44A3-8807-9EF7030F3290}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE2443D-209A-40FF-BEB7-471594C0AF5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="39">
   <si>
     <t>Item</t>
   </si>
@@ -154,6 +154,9 @@
   </si>
   <si>
     <t>Sprint 2</t>
+  </si>
+  <si>
+    <t>Sprint 3</t>
   </si>
 </sst>
 </file>
@@ -176,7 +179,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -198,12 +201,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -253,7 +250,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -271,16 +268,10 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -423,10 +414,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>156</c:v>
+                  <c:v>151</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>184</c:v>
+                  <c:v>113</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -469,10 +460,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>19</c:v>
+                  <c:v>85</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>47</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -485,7 +476,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -1533,10 +1523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:H24"/>
+  <dimension ref="B2:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1599,50 +1589,50 @@
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="5">
+      <c r="B4" s="2">
         <f>B3+1</f>
         <v>2</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="2">
         <v>13</v>
       </c>
-      <c r="G4" s="5">
-        <v>1</v>
-      </c>
-      <c r="H4" s="5">
+      <c r="G4" s="2">
+        <v>1</v>
+      </c>
+      <c r="H4" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="5">
+      <c r="B5" s="2">
         <f t="shared" ref="B5:B19" si="0">B4+1</f>
         <v>3</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="2">
         <v>3</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="2">
         <v>3</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="2">
         <v>1</v>
       </c>
     </row>
@@ -1695,363 +1685,382 @@
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="5">
+      <c r="B8" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="2">
         <v>21</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="2">
         <v>2</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="7">
+      <c r="B9" s="5">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="5">
         <v>8</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="5">
         <v>3</v>
       </c>
-      <c r="H9" s="7">
+      <c r="H9" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="7">
+      <c r="B10" s="5">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="5">
         <v>8</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="5">
         <v>3</v>
       </c>
-      <c r="H10" s="7">
+      <c r="H10" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="7">
+      <c r="B11" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="7">
-        <v>13</v>
-      </c>
-      <c r="G11" s="7">
-        <v>1</v>
-      </c>
-      <c r="H11" s="7">
+      <c r="E11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="2">
+        <v>8</v>
+      </c>
+      <c r="G11" s="2">
+        <v>1</v>
+      </c>
+      <c r="H11" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="7">
+      <c r="B12" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="2">
         <v>21</v>
       </c>
-      <c r="G12" s="7">
-        <v>1</v>
-      </c>
-      <c r="H12" s="7">
+      <c r="G12" s="2">
+        <v>1</v>
+      </c>
+      <c r="H12" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="7">
+      <c r="B13" s="5">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="5">
         <v>21</v>
       </c>
-      <c r="G13" s="7">
-        <v>1</v>
-      </c>
-      <c r="H13" s="7">
+      <c r="G13" s="5">
+        <v>1</v>
+      </c>
+      <c r="H13" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="7">
+      <c r="B14" s="5">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="5">
         <v>8</v>
       </c>
-      <c r="G14" s="7">
-        <v>1</v>
-      </c>
-      <c r="H14" s="7">
+      <c r="G14" s="5">
+        <v>1</v>
+      </c>
+      <c r="H14" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="7">
+      <c r="B15" s="5">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="5">
         <v>21</v>
       </c>
-      <c r="G15" s="7">
-        <v>1</v>
-      </c>
-      <c r="H15" s="7">
+      <c r="G15" s="5">
+        <v>1</v>
+      </c>
+      <c r="H15" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="7">
+      <c r="B16" s="5">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E16" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F16" s="5">
         <v>13</v>
       </c>
-      <c r="G16" s="7">
-        <v>1</v>
-      </c>
-      <c r="H16" s="7">
+      <c r="G16" s="5">
+        <v>1</v>
+      </c>
+      <c r="H16" s="5">
         <v>2</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="7">
+      <c r="B17" s="5">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E17" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="5">
         <v>13</v>
       </c>
-      <c r="G17" s="7">
-        <v>1</v>
-      </c>
-      <c r="H17" s="7">
+      <c r="G17" s="5">
+        <v>1</v>
+      </c>
+      <c r="H17" s="5">
         <v>2</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="7">
+      <c r="B18" s="5">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="E18" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F18" s="5">
         <v>8</v>
       </c>
-      <c r="G18" s="7">
+      <c r="G18" s="5">
         <v>3</v>
       </c>
-      <c r="H18" s="7">
+      <c r="H18" s="5">
         <v>2</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="7">
+      <c r="B19" s="5">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E19" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F19" s="5">
         <v>13</v>
       </c>
-      <c r="G19" s="7">
+      <c r="G19" s="5">
         <v>3</v>
       </c>
-      <c r="H19" s="7">
+      <c r="H19" s="5">
         <v>2</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="12"/>
-      <c r="C21" s="12" t="s">
+      <c r="B21" s="10"/>
+      <c r="C21" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="D21" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="E21" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="F21" s="11" t="s">
+      <c r="F21" s="9" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="12">
+      <c r="C22" s="10">
         <f>SUM(C23,C24)</f>
+        <v>198</v>
+      </c>
+      <c r="D22" s="8">
         <v>203</v>
       </c>
-      <c r="D22" s="10">
-        <v>203</v>
-      </c>
-      <c r="E22" s="9">
+      <c r="E22" s="7">
         <f>SUM(E23,E24)</f>
+        <v>85</v>
+      </c>
+      <c r="F22" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="10">
+        <f>SUM(F3:F15)</f>
+        <v>151</v>
+      </c>
+      <c r="D23" s="8">
+        <f>SUM(C23+F22)</f>
+        <v>151</v>
+      </c>
+      <c r="E23" s="7">
+        <v>85</v>
+      </c>
+      <c r="F23" s="9">
+        <f>D23-E23</f>
         <v>66</v>
       </c>
-      <c r="F22" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C23" s="12">
-        <f>SUM(F3:F15)</f>
-        <v>156</v>
-      </c>
-      <c r="D23" s="10">
-        <f>SUM(C23+F22)</f>
-        <v>156</v>
-      </c>
-      <c r="E23" s="9">
-        <v>19</v>
-      </c>
-      <c r="F23" s="11">
-        <f>D23-E23</f>
-        <v>137</v>
-      </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="12" t="s">
+      <c r="B24" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C24" s="12">
+      <c r="C24" s="10">
         <f>SUM(F16:F19)</f>
         <v>47</v>
       </c>
-      <c r="D24" s="10">
+      <c r="D24" s="8">
         <f>SUM(C24+F23)</f>
-        <v>184</v>
-      </c>
-      <c r="E24" s="9">
-        <v>47</v>
-      </c>
-      <c r="F24" s="11">
+        <v>113</v>
+      </c>
+      <c r="E24" s="7">
+        <v>0</v>
+      </c>
+      <c r="F24" s="9">
+        <f>(D24-E24)</f>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="10">
+        <v>0</v>
+      </c>
+      <c r="D25" s="8">
+        <f>SUM(C25+F24)</f>
+        <v>113</v>
+      </c>
+      <c r="E25" s="7">
+        <v>0</v>
+      </c>
+      <c r="F25" s="9">
         <v>0</v>
       </c>
     </row>

</xml_diff>